<commit_message>
finalizando alterações na documentação
</commit_message>
<xml_diff>
--- a/planilha de resultados.xlsx
+++ b/planilha de resultados.xlsx
@@ -8,15 +8,13 @@
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
-    <sheet name="Plan2" sheetId="2" r:id="rId2"/>
-    <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
   <si>
     <t>numeroMaxIteracao</t>
   </si>
@@ -28,6 +26,9 @@
   </si>
   <si>
     <t>avioesCaidos</t>
+  </si>
+  <si>
+    <t>DEPOIS DA REFATORAÇÃO PARA CAIR MENOS AVIÕES</t>
   </si>
 </sst>
 </file>
@@ -59,7 +60,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -67,21 +68,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -385,28 +407,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D17" sqref="A13:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
@@ -414,75 +436,138 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+      <c r="A2" s="6">
         <v>100</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1">
+      <c r="B2" s="6">
+        <v>173</v>
+      </c>
+      <c r="C2" s="6">
+        <v>123</v>
+      </c>
+      <c r="D2" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="A3" s="7">
         <v>1000</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1">
+      <c r="B3" s="7">
+        <v>1810</v>
+      </c>
+      <c r="C3" s="7">
+        <v>1109</v>
+      </c>
+      <c r="D3" s="6">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="A4" s="7">
         <v>10000</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1">
-        <v>127</v>
+      <c r="B4" s="7">
+        <v>18201</v>
+      </c>
+      <c r="C4" s="7">
+        <v>11103</v>
+      </c>
+      <c r="D4" s="6">
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="A5" s="7">
         <v>100000</v>
       </c>
-      <c r="B5" s="3">
-        <v>175600</v>
-      </c>
-      <c r="C5" s="3">
-        <v>122950</v>
-      </c>
-      <c r="D5" s="1">
-        <v>640</v>
+      <c r="B5" s="7">
+        <v>175804</v>
+      </c>
+      <c r="C5" s="7">
+        <v>122945</v>
+      </c>
+      <c r="D5" s="6">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
+        <v>100</v>
+      </c>
+      <c r="B14" s="6">
+        <v>198</v>
+      </c>
+      <c r="C14" s="6">
+        <v>102</v>
+      </c>
+      <c r="D14" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
+        <v>1000</v>
+      </c>
+      <c r="B15" s="7">
+        <v>1977</v>
+      </c>
+      <c r="C15" s="6">
+        <v>937</v>
+      </c>
+      <c r="D15" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
+        <v>10000</v>
+      </c>
+      <c r="B16" s="7">
+        <v>19846</v>
+      </c>
+      <c r="C16" s="6">
+        <v>9791</v>
+      </c>
+      <c r="D16" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
+        <v>100000</v>
+      </c>
+      <c r="B17" s="7">
+        <v>198199</v>
+      </c>
+      <c r="C17" s="7">
+        <v>101259</v>
+      </c>
+      <c r="D17" s="6">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>